<commit_message>
ContractTemplate: import xlsx  spreadsheets
</commit_message>
<xml_diff>
--- a/docs/ContractTemplate.xlsx
+++ b/docs/ContractTemplate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\node\Contractzlab-api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E4E639-EE3B-4973-A57D-B474E568EF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E35B9E-642E-4F4A-BF3C-83ECF200D3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Saas" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Saas" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="122">
   <si>
     <t>Doc_code</t>
   </si>
@@ -407,6 +408,36 @@
     <t>$tacite[Le Contrat sera prorogé par tacite prorogation pour des périodes identiques sauf décision de l’une ou l’autre des Parties de mettre fin au Contrat par l’envoi d’une lettre recommandée avec demande d’avis de réception, $Preavis jours avant la date anniversaire du Contrat (date de la première présentation par les services de La Poste).][
 Le Contrat sera pas prorogé par tacite prorogation]</t>
   </si>
+  <si>
+    <t>FAKE_1</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Contrat Service</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>FAKE_1.1</t>
+  </si>
+  <si>
+    <t>FAKE_1.2</t>
+  </si>
+  <si>
+    <t>FAKE_1.3</t>
+  </si>
+  <si>
+    <t>FAKE_1.4</t>
+  </si>
+  <si>
+    <t>FAKE_1.5</t>
+  </si>
+  <si>
+    <t>FAKE_1.6</t>
+  </si>
 </sst>
 </file>
 
@@ -588,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -684,16 +715,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -703,11 +736,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,12 +957,903 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9ADFEE5-83AE-424A-A084-4F13A6DDB389}">
+  <dimension ref="A1:AK14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12:K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="33">
+        <v>1</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="36"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="U2" s="8">
+        <v>1</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+    </row>
+    <row r="3" spans="1:37" ht="344.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+    </row>
+    <row r="4" spans="1:37" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+    </row>
+    <row r="5" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="8">
+        <v>2</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK5" s="8"/>
+    </row>
+    <row r="6" spans="1:37" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="33">
+        <v>3</v>
+      </c>
+      <c r="M6" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="U6" s="8"/>
+      <c r="V6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+    </row>
+    <row r="7" spans="1:37" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" s="8"/>
+      <c r="V7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+    </row>
+    <row r="8" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="T8" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="U8" s="32"/>
+      <c r="V8" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB8" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC8" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="16"/>
+      <c r="AI8" s="32"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="32"/>
+    </row>
+    <row r="9" spans="1:37" ht="283.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="L9" s="33">
+        <v>4</v>
+      </c>
+      <c r="M9" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="U9" s="19"/>
+      <c r="V9" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="19"/>
+      <c r="AE9" s="19"/>
+      <c r="AF9" s="19"/>
+      <c r="AG9" s="19"/>
+      <c r="AH9" s="19"/>
+      <c r="AI9" s="19"/>
+      <c r="AJ9" s="19"/>
+      <c r="AK9" s="19"/>
+    </row>
+    <row r="10" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24">
+        <v>4.2</v>
+      </c>
+      <c r="T10" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="U10" s="24"/>
+      <c r="V10" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z10" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA10" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="24"/>
+      <c r="AJ10" s="24"/>
+      <c r="AK10" s="24"/>
+    </row>
+    <row r="11" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L11" s="8">
+        <v>5</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z11" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA11" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="21"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="21"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="21"/>
+      <c r="AK11" s="21"/>
+    </row>
+    <row r="12" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="33">
+        <v>6</v>
+      </c>
+      <c r="M12" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21">
+        <v>6.1</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="21"/>
+      <c r="AD12" s="21"/>
+      <c r="AE12" s="21"/>
+      <c r="AF12" s="21"/>
+      <c r="AG12" s="21"/>
+      <c r="AH12" s="21"/>
+      <c r="AI12" s="21"/>
+      <c r="AJ12" s="21"/>
+      <c r="AK12" s="21"/>
+    </row>
+    <row r="13" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21">
+        <v>6.2</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="21"/>
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="21"/>
+      <c r="AG13" s="21"/>
+      <c r="AH13" s="21"/>
+      <c r="AI13" s="21"/>
+      <c r="AJ13" s="21"/>
+      <c r="AK13" s="21"/>
+    </row>
+    <row r="14" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21">
+        <v>6.3</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="21"/>
+      <c r="AC14" s="21"/>
+      <c r="AD14" s="21"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="21"/>
+      <c r="AG14" s="21"/>
+      <c r="AH14" s="21"/>
+      <c r="AI14" s="21"/>
+      <c r="AJ14" s="21"/>
+      <c r="AK14" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="G2:G14"/>
+    <mergeCell ref="H2:H14"/>
+    <mergeCell ref="I2:I14"/>
+    <mergeCell ref="J2:J14"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C2:C14"/>
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="E2:E14"/>
+    <mergeCell ref="F2:F14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1081,41 +2006,41 @@
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="33">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="34">
+      <c r="K2" s="37">
         <v>2.1</v>
       </c>
-      <c r="L2" s="32">
+      <c r="L2" s="33">
         <v>1</v>
       </c>
       <c r="M2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="43"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
       <c r="R2" s="5" t="s">
         <v>42</v>
       </c>
@@ -1163,23 +2088,23 @@
       <c r="AL2" s="9"/>
     </row>
     <row r="3" spans="1:38" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5">
         <v>1.2</v>
@@ -1213,23 +2138,23 @@
       <c r="AL3" s="9"/>
     </row>
     <row r="4" spans="1:38" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5">
         <v>1.3</v>
@@ -1263,16 +2188,16 @@
       <c r="AL4" s="9"/>
     </row>
     <row r="5" spans="1:38" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
       <c r="K5" s="11">
         <v>2.2000000000000002</v>
       </c>
@@ -1335,29 +2260,29 @@
       <c r="AL5" s="9"/>
     </row>
     <row r="6" spans="1:38" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="32">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="33">
         <v>3</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5" t="s">
         <v>67</v>
@@ -1391,23 +2316,23 @@
       <c r="AL6" s="9"/>
     </row>
     <row r="7" spans="1:38" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="40"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5" t="s">
         <v>72</v>
@@ -1449,23 +2374,23 @@
       <c r="AL7" s="9"/>
     </row>
     <row r="8" spans="1:38" ht="195" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
       <c r="K8" s="41"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4" t="s">
         <v>78</v>
@@ -1507,29 +2432,29 @@
       <c r="AL8" s="9"/>
     </row>
     <row r="9" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="34">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="37">
         <v>2.4</v>
       </c>
-      <c r="L9" s="32">
+      <c r="L9" s="33">
         <v>4</v>
       </c>
       <c r="M9" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
       <c r="R9" s="19"/>
       <c r="S9" s="19">
         <v>4.0999999999999996</v>
@@ -1565,23 +2490,23 @@
       <c r="AL9" s="22"/>
     </row>
     <row r="10" spans="1:38" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
       <c r="R10" s="23"/>
       <c r="S10" s="23">
         <v>4.2</v>
@@ -1617,16 +2542,16 @@
       <c r="AL10" s="25"/>
     </row>
     <row r="11" spans="1:38" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="11">
         <v>2.5</v>
       </c>
@@ -1671,29 +2596,29 @@
       <c r="AL11" s="25"/>
     </row>
     <row r="12" spans="1:38" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="37">
         <v>2.6</v>
       </c>
-      <c r="L12" s="32">
+      <c r="L12" s="33">
         <v>6</v>
       </c>
       <c r="M12" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
       <c r="R12" s="21"/>
       <c r="S12" s="21">
         <v>6.1</v>
@@ -1723,23 +2648,23 @@
       <c r="AL12" s="25"/>
     </row>
     <row r="13" spans="1:38" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
       <c r="R13" s="21"/>
       <c r="S13" s="21">
         <v>6.2</v>
@@ -1769,23 +2694,23 @@
       <c r="AL13" s="25"/>
     </row>
     <row r="14" spans="1:38" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
       <c r="R14" s="21"/>
       <c r="S14" s="21">
         <v>6.3</v>
@@ -41254,11 +42179,25 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="B2:B14"/>
-    <mergeCell ref="C2:C14"/>
-    <mergeCell ref="D2:D14"/>
-    <mergeCell ref="E2:E14"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M6:M8"/>
     <mergeCell ref="F2:F14"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -41273,25 +42212,11 @@
     <mergeCell ref="H2:H14"/>
     <mergeCell ref="I2:I14"/>
     <mergeCell ref="J2:J14"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="P6:P8"/>
-    <mergeCell ref="Q6:Q8"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="Q12:Q14"/>
-    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C2:C14"/>
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="E2:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
TypeLevels: optional level3 level2
</commit_message>
<xml_diff>
--- a/docs/ContractTemplate.xlsx
+++ b/docs/ContractTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\node\Contractzlab-api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E35B9E-642E-4F4A-BF3C-83ECF200D3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36964425-A1D2-48C2-8BB2-85F2DC9D13CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="122">
   <si>
     <t>Doc_code</t>
   </si>
@@ -412,9 +412,6 @@
     <t>FAKE_1</t>
   </si>
   <si>
-    <t>Service</t>
-  </si>
-  <si>
     <t>Contrat Service</t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>FAKE_1.6</t>
+  </si>
+  <si>
+    <t>FAKE_TYPE_1</t>
   </si>
 </sst>
 </file>
@@ -715,19 +715,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -736,13 +739,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9ADFEE5-83AE-424A-A084-4F13A6DDB389}">
   <dimension ref="A1:AK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1080,41 +1080,37 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="33" t="s">
+      <c r="G2" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="K2" s="37" t="s">
-        <v>116</v>
+      <c r="H2" s="37" t="s">
+        <v>121</v>
       </c>
-      <c r="L2" s="33">
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="37">
         <v>1</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
       <c r="R2" s="8" t="s">
         <v>42</v>
       </c>
@@ -1122,7 +1118,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U2" s="8">
         <v>1</v>
@@ -1175,7 +1171,7 @@
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
-      <c r="K3" s="38"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
       <c r="N3" s="34"/>
@@ -1224,7 +1220,7 @@
       <c r="H4" s="34"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="44"/>
       <c r="L4" s="35"/>
       <c r="M4" s="35"/>
       <c r="N4" s="35"/>
@@ -1274,7 +1270,7 @@
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
       <c r="K5" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L5" s="8">
         <v>2</v>
@@ -1344,19 +1340,19 @@
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
-      <c r="K6" s="33" t="s">
-        <v>118</v>
+      <c r="K6" s="37" t="s">
+        <v>117</v>
       </c>
-      <c r="L6" s="33">
+      <c r="L6" s="37">
         <v>3</v>
       </c>
       <c r="M6" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8" t="s">
         <v>67</v>
@@ -1399,7 +1395,7 @@
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
-      <c r="K7" s="40"/>
+      <c r="K7" s="41"/>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
@@ -1456,7 +1452,7 @@
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
-      <c r="K8" s="41"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
@@ -1513,19 +1509,19 @@
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
-      <c r="K9" s="37" t="s">
-        <v>119</v>
+      <c r="K9" s="38" t="s">
+        <v>118</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="37">
         <v>4</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
       <c r="R9" s="19"/>
       <c r="S9" s="19">
         <v>4.0999999999999996</v>
@@ -1570,7 +1566,7 @@
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
-      <c r="K10" s="38"/>
+      <c r="K10" s="39"/>
       <c r="L10" s="34"/>
       <c r="M10" s="35"/>
       <c r="N10" s="34"/>
@@ -1622,7 +1618,7 @@
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
       <c r="K11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L11" s="8">
         <v>5</v>
@@ -1674,19 +1670,19 @@
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
-      <c r="K12" s="37" t="s">
-        <v>121</v>
+      <c r="K12" s="38" t="s">
+        <v>120</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="37">
         <v>6</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
       <c r="R12" s="21"/>
       <c r="S12" s="21">
         <v>6.1</v>
@@ -1725,7 +1721,7 @@
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
-      <c r="K13" s="38"/>
+      <c r="K13" s="39"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
@@ -1770,7 +1766,7 @@
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
-      <c r="K14" s="42"/>
+      <c r="K14" s="44"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
@@ -1804,11 +1800,25 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C2:C14"/>
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="E2:E14"/>
+    <mergeCell ref="F2:F14"/>
+    <mergeCell ref="G2:G14"/>
+    <mergeCell ref="H2:H14"/>
+    <mergeCell ref="I2:I14"/>
+    <mergeCell ref="J2:J14"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
     <mergeCell ref="P6:P8"/>
     <mergeCell ref="Q6:Q8"/>
     <mergeCell ref="K9:K10"/>
@@ -1818,30 +1828,16 @@
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="Q2:Q4"/>
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="L6:L8"/>
     <mergeCell ref="M6:M8"/>
     <mergeCell ref="N6:N8"/>
     <mergeCell ref="O6:O8"/>
-    <mergeCell ref="G2:G14"/>
-    <mergeCell ref="H2:H14"/>
-    <mergeCell ref="I2:I14"/>
-    <mergeCell ref="J2:J14"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="B2:B14"/>
-    <mergeCell ref="C2:C14"/>
-    <mergeCell ref="D2:D14"/>
-    <mergeCell ref="E2:E14"/>
-    <mergeCell ref="F2:F14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2006,41 +2002,41 @@
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
+      <c r="A2" s="37">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="38">
         <v>2.1</v>
       </c>
-      <c r="L2" s="33">
+      <c r="L2" s="37">
         <v>1</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
       <c r="R2" s="5" t="s">
         <v>42</v>
       </c>
@@ -2098,7 +2094,7 @@
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
-      <c r="K3" s="38"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
       <c r="N3" s="34"/>
@@ -2148,7 +2144,7 @@
       <c r="H4" s="34"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="44"/>
       <c r="L4" s="35"/>
       <c r="M4" s="35"/>
       <c r="N4" s="35"/>
@@ -2270,19 +2266,19 @@
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
-      <c r="K6" s="33">
+      <c r="K6" s="37">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L6" s="33">
+      <c r="L6" s="37">
         <v>3</v>
       </c>
       <c r="M6" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5" t="s">
         <v>67</v>
@@ -2326,7 +2322,7 @@
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
-      <c r="K7" s="40"/>
+      <c r="K7" s="41"/>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
@@ -2384,7 +2380,7 @@
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
-      <c r="K8" s="41"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
@@ -2442,19 +2438,19 @@
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
-      <c r="K9" s="37">
+      <c r="K9" s="38">
         <v>2.4</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="37">
         <v>4</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
       <c r="R9" s="19"/>
       <c r="S9" s="19">
         <v>4.0999999999999996</v>
@@ -2500,7 +2496,7 @@
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
-      <c r="K10" s="38"/>
+      <c r="K10" s="39"/>
       <c r="L10" s="34"/>
       <c r="M10" s="35"/>
       <c r="N10" s="34"/>
@@ -2606,19 +2602,19 @@
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
-      <c r="K12" s="37">
+      <c r="K12" s="38">
         <v>2.6</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="37">
         <v>6</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
       <c r="R12" s="21"/>
       <c r="S12" s="21">
         <v>6.1</v>
@@ -2658,7 +2654,7 @@
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
-      <c r="K13" s="38"/>
+      <c r="K13" s="39"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
@@ -2704,7 +2700,7 @@
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
-      <c r="K14" s="42"/>
+      <c r="K14" s="44"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
@@ -42179,25 +42175,11 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="Q12:Q14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="P6:P8"/>
-    <mergeCell ref="Q6:Q8"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C2:C14"/>
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="E2:E14"/>
     <mergeCell ref="F2:F14"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -42212,11 +42194,25 @@
     <mergeCell ref="H2:H14"/>
     <mergeCell ref="I2:I14"/>
     <mergeCell ref="J2:J14"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="B2:B14"/>
-    <mergeCell ref="C2:C14"/>
-    <mergeCell ref="D2:D14"/>
-    <mergeCell ref="E2:E14"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="M12:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>